<commit_message>
Content new Changes for Factory and Madewell
</commit_message>
<xml_diff>
--- a/desktop-functional-tests/ContentTestingSheet/Content_testing_template_Jcrew.xlsx
+++ b/desktop-functional-tests/ContentTestingSheet/Content_testing_template_Jcrew.xlsx
@@ -443,7 +443,7 @@
     <t>https://factory.jcrew.com/c/boys_shops/online_exclusives</t>
   </si>
   <si>
-    <t/>
+    <t>Respose code</t>
   </si>
 </sst>
 </file>
@@ -1186,8 +1186,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K903"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1195,6 +1195,7 @@
     <col min="1" max="1" width="41.85546875" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="58.7109375" customWidth="1" collapsed="1"/>
     <col min="3" max="3" width="16.140625" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="13.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="18.28515625" customWidth="1" collapsed="1"/>
     <col min="6" max="6" width="24.5703125" customWidth="1" collapsed="1"/>
   </cols>

</xml_diff>

<commit_message>
contact centre orders(100 tests)
</commit_message>
<xml_diff>
--- a/desktop-functional-tests/ContentTestingSheet/Content_testing_template_Jcrew.xlsx
+++ b/desktop-functional-tests/ContentTestingSheet/Content_testing_template_Jcrew.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18201"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Desktop\sidecar-functional-tests\desktop-functional-tests\ContentTestingSheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15270" windowHeight="5865"/>
+    <workbookView windowHeight="5865" windowWidth="15270" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Home" sheetId="1" r:id="rId1"/>
+    <sheet name="Home" r:id="rId1" sheetId="1"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -39,6 +39,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="0"/>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -109,23 +110,23 @@
     </border>
   </borders>
   <cellStyleXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="4">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" applyFont="1" borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="3" numFmtId="49" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Excel Built-in Normal" xfId="1"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -142,10 +143,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -180,7 +181,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin panose="020F0302020204030204" typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -215,7 +216,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -309,21 +310,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -340,7 +341,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -392,15 +393,15 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
@@ -408,11 +409,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="41.85546875" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="58.7109375" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="23.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="18.28515625" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="24.5703125" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="41.85546875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="58.7109375" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="23.7109375" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="18.28515625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="24.5703125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -479,9 +480,9 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B3" r:id="rId1" display="https://or.jcrew.com/r/login"/>
+    <hyperlink display="https://or.jcrew.com/r/login" r:id="rId1" ref="B3"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" r:id="rId2"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="4294967293" orientation="portrait" paperSize="9" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>